<commit_message>
Fix load file soi initiation
</commit_message>
<xml_diff>
--- a/station_in_config/Line.xlsx
+++ b/station_in_config/Line.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="450" windowWidth="7335" windowHeight="8385"/>
+    <workbookView xWindow="11370" yWindow="465" windowWidth="7335" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,14 +61,14 @@
     <t>Point_16 Point_12</t>
   </si>
   <si>
-    <t>Point_18 Point_20</t>
+    <t>Point_18 Point_20 Point_15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +128,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -415,19 +420,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -443,7 +448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -451,7 +456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -459,7 +464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -467,7 +472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -475,7 +480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -483,7 +488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Read station config method begin
</commit_message>
<xml_diff>
--- a/station_in_config/Line.xlsx
+++ b/station_in_config/Line.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="165" windowWidth="7335" windowHeight="4170"/>
+    <workbookView xWindow="1665" yWindow="150" windowWidth="13605" windowHeight="4170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,26 +421,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -448,7 +450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -456,7 +458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -464,7 +466,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -472,7 +474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -480,7 +482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -488,7 +490,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>

</xml_diff>